<commit_message>
Graphs for ndcg and precision
</commit_message>
<xml_diff>
--- a/result-metric-I/Final.xlsx
+++ b/result-metric-I/Final.xlsx
@@ -5,13 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="IR" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="P@i" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="WSN" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="SE" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="PDS" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="AI" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="CV" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="mm" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Security" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="NLP" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="ML" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="IP" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="DM" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="5">
   <si>
     <t xml:space="preserve">Snaver</t>
   </si>
@@ -47,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -80,6 +89,14 @@
     </font>
     <font>
       <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -129,7 +146,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -143,6 +160,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,14 +186,14 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="25" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,6 +404,924 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.9234824915</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.944971889</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.833333333333333</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.85671355</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.929809757</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.873302077666667</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.826363638</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.932020136</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.787070704333333</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.786899094666667</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.9037849785</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.792664874333333</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.791448518666667</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.8933876575</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.763990846</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.794914448666667</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.8720446445</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.755937359333333</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.820314013333333</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.874077925</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.747409953</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.819313018</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.9378254925</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.736916277666667</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.809360695</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.962511563</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.728046623666667</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.824793900666667</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.720693811</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.829617184333333</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.734194076666667</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.841317795</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.754187557333333</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.850698588</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.773454377333333</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.87678723</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.792315479333333</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.900945807666667</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.810264169666667</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.902278707666667</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.834642481</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.902278707666667</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.857561229</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.908223945</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.870986067333333</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.919910829666667</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.890940166</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.816744805666667</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.769984372333333</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.792777781333333</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.780101009333333</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.693282828666667</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.797681839666667</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.776900839</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.669910682333333</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.817504091</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.770677466666667</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.653263574666667</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.832605459666667</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.765536279666667</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.654372668</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.844636116333333</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.824777053333333</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.67504034</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.822687722666667</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.865885649333333</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.678372395333333</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.813749276333333</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.879380644333333</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.680949663333333</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.814770472333333</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.673516384666667</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.820846437</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.692008403</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.834065710666667</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.715783161333333</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.846233386333334</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.738051486</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.857105570666667</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.751184376</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.87239483</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.767874558</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.881251407</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.789843900666667</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.877679332666667</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.803610878</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.896151895333333</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.824100542333333</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.924642887333333</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.844030023</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.79166666675</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.60416666675</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.8150468835</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.74619399525</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.587147052</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.82462121425</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.80010825675</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.53232330725</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.81559786825</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.80079500775</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.527822617</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.82141782975</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.808267483</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.51734146125</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.80516443475</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.8301773065</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.51083095225</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.81916727925</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.81364739575</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.5012245935</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.8227230255</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.87380610325</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.510860323</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.82571797325</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.89726886475</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.5196772955</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.81525168225</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.541911727</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.8170417945</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.54925850325</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.82787786925</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.567177772</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.8317181785</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.60413233225</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.8403275935</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.62836341525</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.853328709</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.652534833</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.86063283625</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.69885519575</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.88139181825</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.71524121325</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.896655911</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.7219167525</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.9228027425</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.740124038</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.95248827925</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.95248827925</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.63501443675</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.960075757</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.9566112295</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.584634383</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.9649034765</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.96190048975</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.574710261</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.96834208075</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.92225538225</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.54704489325</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.9709617445</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.92751134525</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.54980998825</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.96406496775</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.927569618</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.56228327475</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.96635351575</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.947240996</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.5480752695</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.96828112275</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.9570027735</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.56488907875</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.96321583725</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.5919091125</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.96480270025</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.6218866275</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.96025549725</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.6304378865</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.956483416</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.64782483075</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.9579453395</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.662582721</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.94500916475</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.70090051925</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.94617044025</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.724360936</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.96024012875</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.74082590225</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.97344108075</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.760004478</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.9822641655</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.764900412925</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -401,7 +1340,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="26" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +1789,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="26" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,7 +2018,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="26" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,4 +2231,1146 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.690046884</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.404976559</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.529282571</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.699621215</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.420151514</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.588532252</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.735943618</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.399576453</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.628248836</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.737320801</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.419199947</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.636427112</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.717682723</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.422263356</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.66588761</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.750546831</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.444342311</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.710420293</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.761988999</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.464544087</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.748893469</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.771884401</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.449069347</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.767249838</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.78221892</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.489134953</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.790175785</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.495749218</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.810306085</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.523406492</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.814670221</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.580079145</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.807009181</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.580079145</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.811070755</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.608436352</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.824150379</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.648706043</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.83649675</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.662306867</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.848184184</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.675657946</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.884571902</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.688780426</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.680093767</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.47561488</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.611309155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.683272732</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.506071722</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.610207098</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.649018826</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.532330534</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.562954222</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.69045727</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.586827444</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.600202604</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.714752592</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.611481652</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.612387521</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.716638913</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.604865714</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.669496712</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.718014838</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.605446459</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.732214855</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.72868614</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.618506056</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.760863159</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.75485488</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.642925233</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.758518828</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.665818316</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.764540341</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.656790094</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.779351763</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.653288161</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.788443818</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.656037841</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.792504959</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.659533924</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.798858271</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.679923569</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.829088965</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.694259503</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.84237466</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.72432577</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.86939161</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.743379696</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.8099531166</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.8760187532</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.8321312732</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.8083636342</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.8583355444</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.7950606118</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.8315366866</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.8442160832</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.7835656928</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.8480419874</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.8324217802</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.7829677872</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.8606163736</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.8678385016</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.7881900606</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.856259871</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.88592575</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.8059731854</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.8654140622</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.910688162</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.8067504358</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.8731244908</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.9280496112</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.8019273424</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.8693114682</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.8358594682</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.8612001376</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.8418979218</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.8355425564</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.8422423616</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.8335720012</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.870393453</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.8383851738</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.8664745142</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.8493698022</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.8815954668</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.8553826642</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.8815954668</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.8647226706</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.8866483956</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.895556925</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.9039604144</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.9259835132</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.9077798468</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.88597187</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.8040750134</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.732023135</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.8243333312</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.7313075292</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.6904575896</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.8213908962</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.7621964402</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.6731673374</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.8192951094</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.7382967408</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.6591270914</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.8176984568</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.7716031346</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.6413879944</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.823613474</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.8109368526</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.6548759816</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.8197197806</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.836091445</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.6573370792</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.8162171342</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.8825040378</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.6574755788</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.7817481372</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.6572749042</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.795789328</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.664651416</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.8034274618</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.6825577686</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.812038178</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.700827004</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.827408828</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.7398224492</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.837596223</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.7634117148</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.8515236894</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.7690524054</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.869890588</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.7915797974</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.884159158</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.79669574</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.913765133</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.813096157</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.79166666675</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.92251172075</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.81961188925</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.56862612475</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.84525106925</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.58435710725</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.81633184425</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.57355520575</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.85050609025</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.8069232595</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.5664833665</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.8421893035</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.817033574</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.56372875525</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.835563652</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.82102448425</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.57094214025</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.83011447075</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.8650045425</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.58097621625</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.8255247125</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.89958678075</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.59204419</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0.83867145575</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.611170297</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0.84972027025</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.62001392225</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>0.87160621075</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.62001392225</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>0.88538270025</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.62834098</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>0.88241615175</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.64394892675</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>0.8946630005</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.67586971725</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>0.9061862335</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.698213979</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0.907950723</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.705817009</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0.91848275875</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.72110697425</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0.940846752</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.74944993575</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>